<commit_message>
Best Buy manual testing fourth commit
</commit_message>
<xml_diff>
--- a/BestBuy Gift Ideas 2.xlsx
+++ b/BestBuy Gift Ideas 2.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/vishnumolakala-keerthi-bhavani_b_capgemini_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{E5F63719-FC1E-4D41-B5AE-D5ECC53049A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEE1AC93-DA3C-497A-8DB0-C08805BC7E07}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{E5F63719-FC1E-4D41-B5AE-D5ECC53049A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F17DBC4-EF79-40AA-8A06-6DA31FCFA1F8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="4" activeTab="5" xr2:uid="{38FE3EE8-D9BF-4D1F-9E36-E62EA904D0AB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{38FE3EE8-D9BF-4D1F-9E36-E62EA904D0AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="User Story" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Scenarios" sheetId="2" r:id="rId2"/>
-    <sheet name="Test Cases" sheetId="3" r:id="rId3"/>
-    <sheet name="RTM" sheetId="5" r:id="rId4"/>
-    <sheet name="Defect Report" sheetId="4" r:id="rId5"/>
-    <sheet name="Summary" sheetId="7" r:id="rId6"/>
-    <sheet name="Test Execution Summary" sheetId="6" r:id="rId7"/>
+    <sheet name="AUT_Participants_module" sheetId="8" r:id="rId1"/>
+    <sheet name="User Story" sheetId="1" r:id="rId2"/>
+    <sheet name="Test Scenarios" sheetId="2" r:id="rId3"/>
+    <sheet name="Test Cases" sheetId="3" r:id="rId4"/>
+    <sheet name="RTM" sheetId="5" r:id="rId5"/>
+    <sheet name="Defect Report" sheetId="4" r:id="rId6"/>
+    <sheet name="Summary" sheetId="7" r:id="rId7"/>
+    <sheet name="Test Execution Summary" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="277">
   <si>
     <t>High</t>
   </si>
@@ -797,14 +798,144 @@
     <t>Keerthi@capgemini.com</t>
   </si>
   <si>
-    <t>Moderate</t>
+    <t>9. Checkout</t>
+  </si>
+  <si>
+    <t>Out of Scope:</t>
+  </si>
+  <si>
+    <t>Premium gift services</t>
+  </si>
+  <si>
+    <t>Personalized recommendations</t>
+  </si>
+  <si>
+    <t>Wishlist integration</t>
+  </si>
+  <si>
+    <t>Areas not covered:</t>
+  </si>
+  <si>
+    <t>Advanced personalization features</t>
+  </si>
+  <si>
+    <t>4.Test Metrices:</t>
+  </si>
+  <si>
+    <t>Total number of test cases planned:</t>
+  </si>
+  <si>
+    <t>Total number of Test cases Executed:</t>
+  </si>
+  <si>
+    <t>Total number of Test cases Passed:</t>
+  </si>
+  <si>
+    <t>Total number of Test cases Failed:</t>
+  </si>
+  <si>
+    <t>Total number of Test cases Planned</t>
+  </si>
+  <si>
+    <t>Total number of Test cases Executed</t>
+  </si>
+  <si>
+    <t>Total number of Test cases Passed</t>
+  </si>
+  <si>
+    <t>Total number of Test cases Failed</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>[Vishnumolakala Keerthi Bhavani: 11/11/2025 9:16 AM]
+All the test steps were successfully executed, and the expected results were achieved.</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Graphical representation:</t>
+  </si>
+  <si>
+    <t>Requirement Traceability Matrix</t>
+  </si>
+  <si>
+    <t>Batch:</t>
+  </si>
+  <si>
+    <t>V &amp; V Testing Banglore Aug 2025</t>
+  </si>
+  <si>
+    <t>Sprint Date:</t>
+  </si>
+  <si>
+    <t>6th Nov 2025 - 18th Nov 2025</t>
+  </si>
+  <si>
+    <t>Application Under Test:</t>
+  </si>
+  <si>
+    <t>Best Buy</t>
+  </si>
+  <si>
+    <t>Associates Name</t>
+  </si>
+  <si>
+    <t>Module undet test</t>
+  </si>
+  <si>
+    <t>Alluri Soujanya</t>
+  </si>
+  <si>
+    <t>TV &amp; Home Theater</t>
+  </si>
+  <si>
+    <t>BR_BestBuy_TV &amp; Home Theater_01</t>
+  </si>
+  <si>
+    <t>Karri Visalakshi</t>
+  </si>
+  <si>
+    <t>Top Deals</t>
+  </si>
+  <si>
+    <t>BR_BestBuy_TopDeals_02</t>
+  </si>
+  <si>
+    <t>Sripathi Akhila</t>
+  </si>
+  <si>
+    <t>Gift Cards</t>
+  </si>
+  <si>
+    <t>BR_BestBuy_GiftCard_03</t>
+  </si>
+  <si>
+    <t>Sunchu Snehanjali</t>
+  </si>
+  <si>
+    <t>Deal of the Day</t>
+  </si>
+  <si>
+    <t>BR_BestBuy_DealoftheDay_04</t>
+  </si>
+  <si>
+    <t>Vishnumolakala Keerthi Bhavani</t>
+  </si>
+  <si>
+    <t>Gift Ideas</t>
+  </si>
+  <si>
+    <t>Group Leader:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -926,8 +1057,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -994,8 +1169,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1090,30 +1271,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1202,20 +1365,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1255,25 +1460,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1295,6 +1511,60 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>474507</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>160494</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>781539</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>188406</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B820D9EE-2217-E9B4-1AB1-22386677C8AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3461100" y="11534670"/>
+          <a:ext cx="2505109" cy="2805165"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1613,10 +1883,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CC3703-EE66-403A-BE4B-C52D2CE82A96}">
+  <dimension ref="A3:D15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.7265625" customWidth="1"/>
+    <col min="2" max="2" width="62.7265625" customWidth="1"/>
+    <col min="3" max="3" width="72.54296875" customWidth="1"/>
+    <col min="4" max="4" width="79.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="57" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+    </row>
+    <row r="4" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="57" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+    </row>
+    <row r="5" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="57" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>259</v>
+      </c>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="55"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+    </row>
+    <row r="7" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="D7" s="57" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="55">
+        <v>1</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>262</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>263</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="55">
+        <v>2</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>265</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>266</v>
+      </c>
+      <c r="D9" s="55" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="55">
+        <v>3</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>268</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>269</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="55">
+        <v>4</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>271</v>
+      </c>
+      <c r="C11" s="55" t="s">
+        <v>272</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="55">
+        <v>5</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>275</v>
+      </c>
+      <c r="D12" s="55" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="55"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="55"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="57" t="s">
+        <v>276</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>262</v>
+      </c>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E33829A5-338D-4070-9664-41597486BD00}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="104" workbookViewId="0">
+    <sheetView zoomScale="104" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -1642,63 +2075,63 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="63" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="50"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="64"/>
     </row>
     <row r="4" spans="1:4" s="4" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="45"/>
-      <c r="B4" s="44" t="s">
+      <c r="A4" s="59"/>
+      <c r="B4" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="65" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="51"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="65"/>
     </row>
     <row r="6" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="45"/>
-      <c r="B6" s="44" t="s">
+      <c r="A6" s="59"/>
+      <c r="B6" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="63" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="45"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="63"/>
     </row>
     <row r="8" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="45"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="31" t="s">
         <v>153</v>
       </c>
@@ -1710,7 +2143,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="45"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="31" t="s">
         <v>154</v>
       </c>
@@ -1722,7 +2155,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="45"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="31" t="s">
         <v>155</v>
       </c>
@@ -1734,7 +2167,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="45"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="31" t="s">
         <v>156</v>
       </c>
@@ -1746,7 +2179,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" s="4" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="45"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="31" t="s">
         <v>157</v>
       </c>
@@ -1758,7 +2191,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="45"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="31" t="s">
         <v>158</v>
       </c>
@@ -1770,7 +2203,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="46"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="31" t="s">
         <v>159</v>
       </c>
@@ -1800,11 +2233,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8597C90B-721D-4801-9C73-9E58C3227FC2}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2024,12 +2457,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A281DC81-B2DA-400E-AEDC-BED8598AA4AB}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="88" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K16"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="88" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2666,12 +3099,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6F78C9-031C-4157-A07A-8930FFE43610}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+    <sheetView topLeftCell="C8" zoomScale="84" workbookViewId="0">
+      <selection sqref="A1:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2705,7 +3138,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="68" t="s">
         <v>215</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2725,7 +3158,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="56"/>
+      <c r="A3" s="70"/>
       <c r="B3" s="5" t="s">
         <v>187</v>
       </c>
@@ -2743,8 +3176,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="56"/>
-      <c r="B4" s="53" t="s">
+      <c r="A4" s="70"/>
+      <c r="B4" s="67" t="s">
         <v>188</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -2761,8 +3194,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="56"/>
-      <c r="B5" s="53"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="5" t="s">
         <v>165</v>
       </c>
@@ -2777,7 +3210,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="56"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="5" t="s">
         <v>189</v>
       </c>
@@ -2795,7 +3228,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="56"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="5" t="s">
         <v>190</v>
       </c>
@@ -2813,7 +3246,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="56"/>
+      <c r="A8" s="70"/>
       <c r="B8" s="5" t="s">
         <v>191</v>
       </c>
@@ -2831,8 +3264,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="56"/>
-      <c r="B9" s="54" t="s">
+      <c r="A9" s="70"/>
+      <c r="B9" s="68" t="s">
         <v>192</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -2849,8 +3282,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="56"/>
-      <c r="B10" s="55"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="5" t="s">
         <v>169</v>
       </c>
@@ -2865,8 +3298,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="56"/>
-      <c r="B11" s="53" t="s">
+      <c r="A11" s="70"/>
+      <c r="B11" s="67" t="s">
         <v>193</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -2883,8 +3316,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="56"/>
-      <c r="B12" s="53"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="3" t="s">
         <v>170</v>
       </c>
@@ -2899,8 +3332,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="56"/>
-      <c r="B13" s="53"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="3" t="s">
         <v>170</v>
       </c>
@@ -2915,8 +3348,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="56"/>
-      <c r="B14" s="53"/>
+      <c r="A14" s="70"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="3" t="s">
         <v>170</v>
       </c>
@@ -2931,8 +3364,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="56"/>
-      <c r="B15" s="53"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="3" t="s">
         <v>170</v>
       </c>
@@ -2947,7 +3380,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="55"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="5" t="s">
         <v>194</v>
       </c>
@@ -2975,11 +3408,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4C7FA1-DA65-4947-A835-3B9B25BF8E02}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -3044,14 +3477,14 @@
       <c r="F2" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="H2" s="63">
+      <c r="H2" s="39">
         <v>45971</v>
       </c>
       <c r="I2" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3063,154 +3496,908 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6CA66D-B294-4C7E-9C27-35C1F418008C}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:G141"/>
+    <sheetView zoomScale="91" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" style="43" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" customWidth="1"/>
+    <col min="2" max="2" width="23" style="37" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" customWidth="1"/>
     <col min="4" max="4" width="19.6328125" customWidth="1"/>
-    <col min="5" max="5" width="57.36328125" customWidth="1"/>
-    <col min="6" max="6" width="46.81640625" customWidth="1"/>
+    <col min="5" max="5" width="48.453125" customWidth="1"/>
+    <col min="6" max="6" width="48.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.5">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="77" t="s">
         <v>216</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="40" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+    </row>
+    <row r="2" spans="1:7" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="78" t="s">
         <v>222</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="41"/>
-      <c r="G5" s="36"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="40" t="s">
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+    </row>
+    <row r="5" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="63" t="s">
         <v>223</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="42"/>
-      <c r="G7" s="36"/>
-    </row>
-    <row r="8" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B8" s="58" t="s">
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+    </row>
+    <row r="7" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="3"/>
+      <c r="B8" s="76" t="s">
         <v>218</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-    </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B9" s="57" t="s">
+      <c r="C8" s="76"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+    </row>
+    <row r="9" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="79" t="s">
         <v>219</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G9" s="36"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="57"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="79"/>
       <c r="C10" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G10" s="36"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="57"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="79"/>
       <c r="C11" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="G11" s="36"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="57"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="G12" s="36"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="57"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="G13" s="36"/>
-    </row>
-    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.4">
-      <c r="B14" s="57"/>
-      <c r="C14" s="39" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="21.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="3"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="47" t="s">
         <v>228</v>
       </c>
-      <c r="G14" s="36"/>
-    </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.4">
-      <c r="B15" s="57"/>
-      <c r="C15" s="39" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="3"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="47" t="s">
         <v>229</v>
       </c>
-      <c r="G15" s="36"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B16" s="57"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+      <c r="B16" s="79"/>
       <c r="C16" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="G16" s="36"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="57"/>
-      <c r="C17" s="3" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="G17" s="36"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="73" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="74" t="s">
+        <v>238</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="75" t="s">
+        <v>240</v>
+      </c>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="3"/>
+      <c r="B25" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="C25" s="46">
+        <v>15</v>
+      </c>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="3"/>
+      <c r="B26" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="C26" s="46">
+        <v>15</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="3"/>
+      <c r="B27" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="C27" s="46">
+        <v>14</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" ht="32.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="3"/>
+      <c r="B28" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="C28" s="46">
+        <v>1</v>
+      </c>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" ht="32" x14ac:dyDescent="0.35">
+      <c r="A30" s="3"/>
+      <c r="B30" s="42" t="s">
+        <v>245</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>246</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>247</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>248</v>
+      </c>
+      <c r="F30" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="3"/>
+      <c r="B31" s="44">
+        <v>15</v>
+      </c>
+      <c r="C31" s="5">
+        <v>15</v>
+      </c>
+      <c r="D31" s="5">
+        <v>14</v>
+      </c>
+      <c r="E31" s="5">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="3"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="3"/>
+      <c r="B34" s="76" t="s">
+        <v>252</v>
+      </c>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A35" s="3"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="3"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="52"/>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="3"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="3"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A53" s="3"/>
+      <c r="B53" s="72" t="s">
+        <v>253</v>
+      </c>
+      <c r="C53" s="72"/>
+      <c r="D53" s="72"/>
+      <c r="E53" s="72"/>
+      <c r="F53" s="72"/>
+      <c r="G53" s="72"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="3"/>
+      <c r="B54" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="F54" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="G54" s="54" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="3"/>
+      <c r="B55" s="67" t="s">
+        <v>215</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="3"/>
+      <c r="B56" s="67"/>
+      <c r="C56" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="3"/>
+      <c r="B57" s="67"/>
+      <c r="C57" s="67" t="s">
+        <v>188</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="3"/>
+      <c r="B58" s="67"/>
+      <c r="C58" s="67"/>
+      <c r="D58" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="3"/>
+      <c r="B59" s="67"/>
+      <c r="C59" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="3"/>
+      <c r="B60" s="67"/>
+      <c r="C60" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F60" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="3"/>
+      <c r="B61" s="67"/>
+      <c r="C61" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="3"/>
+      <c r="B62" s="67"/>
+      <c r="C62" s="67" t="s">
+        <v>192</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F62" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="3"/>
+      <c r="B63" s="67"/>
+      <c r="C63" s="67"/>
+      <c r="D63" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F63" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="3"/>
+      <c r="B64" s="67"/>
+      <c r="C64" s="67" t="s">
+        <v>193</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F64" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="3"/>
+      <c r="B65" s="67"/>
+      <c r="C65" s="67"/>
+      <c r="D65" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" s="3"/>
+      <c r="B66" s="67"/>
+      <c r="C66" s="67"/>
+      <c r="D66" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F66" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" s="3"/>
+      <c r="B67" s="67"/>
+      <c r="C67" s="67"/>
+      <c r="D67" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F67" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" s="3"/>
+      <c r="B68" s="67"/>
+      <c r="C68" s="67"/>
+      <c r="D68" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F68" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="3"/>
+      <c r="B69" s="67"/>
+      <c r="C69" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F69" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="15">
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B34:F34"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B9:B17"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C6:G6"/>
+    <mergeCell ref="B9:B18"/>
+    <mergeCell ref="C36:D50"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B55:B69"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C64:C68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93B1BD5-59DE-4BC6-9B2C-FFBF099A6047}">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -3232,17 +4419,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="80" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
     </row>
     <row r="2" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">

</xml_diff>